<commit_message>
bổ sung thông tin tra log tác động, fix bug trang danh sách đối tượng, nâng cấp chức năng đăng ký off node bằng excel
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/excel/Template_DELETE_NODE.xlsx
+++ b/src/main/webapp/resources/excel/Template_DELETE_NODE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\RIMS\trunk\code\RIMS\src\main\webapp\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\RIMS\source\RIMS\src\main\webapp\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DC003696-D61E-4D0D-9F06-BEACD712E210}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HUY NODE" sheetId="10" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>A1</t>
   </si>
@@ -53,17 +54,20 @@
   </si>
   <si>
     <t>2GNTN0185</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -100,12 +104,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +136,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -197,7 +215,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,19 +234,22 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 107" xfId="3"/>
-    <cellStyle name="Normal 2 11" xfId="4"/>
-    <cellStyle name="Normal 2 113" xfId="5"/>
-    <cellStyle name="Normal 2 119" xfId="6"/>
-    <cellStyle name="Normal 2 2 10 2" xfId="7"/>
-    <cellStyle name="Normal 2 51" xfId="8"/>
-    <cellStyle name="Normal 2 61" xfId="9"/>
-    <cellStyle name="Normal 2 70" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 107" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 11" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 113" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 119" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 10 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 51" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 61" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 70" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,84 +584,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.25" style="2" customWidth="1"/>
-    <col min="7" max="8" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="19" style="6" customWidth="1"/>
-    <col min="10" max="10" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.375" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.375" customWidth="1"/>
-    <col min="17" max="17" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="F1"/>
-      <c r="I1"/>
+      <c r="D1" s="7"/>
+      <c r="G1"/>
+      <c r="J1"/>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2"/>
-      <c r="I2"/>
+      <c r="G2"/>
+      <c r="J2"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3"/>
-      <c r="I3"/>
+      <c r="G3"/>
+      <c r="J3"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4"/>
-      <c r="I4"/>
+      <c r="G4"/>
+      <c r="J4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,12 +675,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>